<commit_message>
mark papers that are wikipedia only with blank guide source
</commit_message>
<xml_diff>
--- a/Midterm Report/Selection of Prompt Engineering Methods/General Text-to-Text Prompt Engineering Methods.xlsx
+++ b/Midterm Report/Selection of Prompt Engineering Methods/General Text-to-Text Prompt Engineering Methods.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\anlp23-project\Midterm Report\Selection of Prompt Engineering Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11438E1-E49D-4C8C-8748-CEBA6679A159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8CC32A-2AA8-4A8F-B38F-2391F98D63E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Method</t>
   </si>
@@ -232,7 +232,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -267,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,9 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -791,6 +789,9 @@
       <c r="H9" t="s">
         <v>1</v>
       </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1087,6 +1088,9 @@
       <c r="G20" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1106,26 +1110,28 @@
     <hyperlink ref="I12" r:id="rId12" display="https://www.promptingguide.ai/" xr:uid="{B661F1AA-2284-44CD-B9DA-E8BE246E133D}"/>
     <hyperlink ref="I17" r:id="rId13" display="https://www.promptingguide.ai/" xr:uid="{1C07AABE-24AB-4857-8019-C3A848840DB3}"/>
     <hyperlink ref="I18" r:id="rId14" display="https://www.promptingguide.ai/" xr:uid="{7A5EEB13-7E83-4DBC-8430-E4B71505F2CD}"/>
-    <hyperlink ref="I19" r:id="rId15" display="https://www.promptingguide.ai/" xr:uid="{D3CDBE56-DD6E-4EC6-AE14-488FCA835707}"/>
-    <hyperlink ref="B12" r:id="rId16" display="https://arxiv.org/abs/2302.11520" xr:uid="{C3C994F2-78AC-4E3D-9F00-6EDD0DF23090}"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://arxiv.org/abs/2302.08043" xr:uid="{E52FCA35-E4DA-4E37-B21E-3A9A5969AE4E}"/>
-    <hyperlink ref="B6" r:id="rId18" display="https://arxiv.org/abs/2205.10625" xr:uid="{AB9E3F90-8908-4467-B39F-6738334AB4F7}"/>
-    <hyperlink ref="B7" r:id="rId19" display="https://arxiv.org/abs/2203.11171" xr:uid="{7266B56A-0B05-4F1E-ABA5-BA03CFC103C9}"/>
-    <hyperlink ref="B8" r:id="rId20" display="https://arxiv.org/abs/2210.00720" xr:uid="{3DF6AAA1-41DA-49D0-9AB2-F2034B2E8EC5}"/>
-    <hyperlink ref="C7" r:id="rId21" display="https://arxiv.org/abs/2203.11171" xr:uid="{EA10A7EF-28E2-44D9-8F1B-43170A074702}"/>
-    <hyperlink ref="C6" r:id="rId22" display="https://arxiv.org/abs/2205.10625" xr:uid="{A74E64C9-5FFF-46D3-8718-5E4BB6462BCC}"/>
-    <hyperlink ref="B5" r:id="rId23" display="https://arxiv.org/abs/2110.08387" xr:uid="{D8B3FD69-7DBC-4C22-9539-E58398B965D0}"/>
-    <hyperlink ref="B9" r:id="rId24" display="https://arxiv.org/abs/2303.17651" xr:uid="{11C1F1DD-041C-4138-8F53-051C6EBBC66A}"/>
-    <hyperlink ref="B10" r:id="rId25" display="https://arxiv.org/abs/2305.10601" xr:uid="{524E0623-8CA4-4712-A341-7219154F3113}"/>
-    <hyperlink ref="B11" r:id="rId26" display="https://arxiv.org/abs/2205.11822" xr:uid="{D7CB9552-7EBC-4EC4-933F-830C027F04AB}"/>
-    <hyperlink ref="B14" r:id="rId27" display="https://arxiv.org/abs/2211.01910" xr:uid="{6BF1C92E-DC69-4D02-83C7-061E772D6D9D}"/>
-    <hyperlink ref="B17" r:id="rId28" display="https://arxiv.org/abs/2210.03629" xr:uid="{6F4E5908-32E4-45CB-BE3F-4D6CC548C5A0}"/>
-    <hyperlink ref="B20" r:id="rId29" display="https://arxiv.org/abs/2309.11495" xr:uid="{55879B9C-F88C-4F3A-A402-8BC974CA767C}"/>
-    <hyperlink ref="B16" r:id="rId30" display="https://arxiv.org/abs/2302.12246" xr:uid="{3F530D0A-07C0-497A-94FA-2AF4B0CD77F0}"/>
-    <hyperlink ref="B18" r:id="rId31" display="https://arxiv.org/abs/2302.00923" xr:uid="{A617BD54-8B44-4D19-AF1E-144697664151}"/>
-    <hyperlink ref="B4" r:id="rId32" display="https://arxiv.org/abs/2201.11903" xr:uid="{F527D3C7-625E-48F9-8C8F-FEAA499C60A6}"/>
+    <hyperlink ref="B12" r:id="rId15" display="https://arxiv.org/abs/2302.11520" xr:uid="{C3C994F2-78AC-4E3D-9F00-6EDD0DF23090}"/>
+    <hyperlink ref="B19" r:id="rId16" display="https://arxiv.org/abs/2302.08043" xr:uid="{E52FCA35-E4DA-4E37-B21E-3A9A5969AE4E}"/>
+    <hyperlink ref="B6" r:id="rId17" display="https://arxiv.org/abs/2205.10625" xr:uid="{AB9E3F90-8908-4467-B39F-6738334AB4F7}"/>
+    <hyperlink ref="B7" r:id="rId18" display="https://arxiv.org/abs/2203.11171" xr:uid="{7266B56A-0B05-4F1E-ABA5-BA03CFC103C9}"/>
+    <hyperlink ref="B8" r:id="rId19" display="https://arxiv.org/abs/2210.00720" xr:uid="{3DF6AAA1-41DA-49D0-9AB2-F2034B2E8EC5}"/>
+    <hyperlink ref="C7" r:id="rId20" display="https://arxiv.org/abs/2203.11171" xr:uid="{EA10A7EF-28E2-44D9-8F1B-43170A074702}"/>
+    <hyperlink ref="C6" r:id="rId21" display="https://arxiv.org/abs/2205.10625" xr:uid="{A74E64C9-5FFF-46D3-8718-5E4BB6462BCC}"/>
+    <hyperlink ref="B5" r:id="rId22" display="https://arxiv.org/abs/2110.08387" xr:uid="{D8B3FD69-7DBC-4C22-9539-E58398B965D0}"/>
+    <hyperlink ref="B9" r:id="rId23" display="https://arxiv.org/abs/2303.17651" xr:uid="{11C1F1DD-041C-4138-8F53-051C6EBBC66A}"/>
+    <hyperlink ref="B10" r:id="rId24" display="https://arxiv.org/abs/2305.10601" xr:uid="{524E0623-8CA4-4712-A341-7219154F3113}"/>
+    <hyperlink ref="B11" r:id="rId25" display="https://arxiv.org/abs/2205.11822" xr:uid="{D7CB9552-7EBC-4EC4-933F-830C027F04AB}"/>
+    <hyperlink ref="B14" r:id="rId26" display="https://arxiv.org/abs/2211.01910" xr:uid="{6BF1C92E-DC69-4D02-83C7-061E772D6D9D}"/>
+    <hyperlink ref="B17" r:id="rId27" display="https://arxiv.org/abs/2210.03629" xr:uid="{6F4E5908-32E4-45CB-BE3F-4D6CC548C5A0}"/>
+    <hyperlink ref="B20" r:id="rId28" display="https://arxiv.org/abs/2309.11495" xr:uid="{55879B9C-F88C-4F3A-A402-8BC974CA767C}"/>
+    <hyperlink ref="B16" r:id="rId29" display="https://arxiv.org/abs/2302.12246" xr:uid="{3F530D0A-07C0-497A-94FA-2AF4B0CD77F0}"/>
+    <hyperlink ref="B18" r:id="rId30" display="https://arxiv.org/abs/2302.00923" xr:uid="{A617BD54-8B44-4D19-AF1E-144697664151}"/>
+    <hyperlink ref="B4" r:id="rId31" display="https://arxiv.org/abs/2201.11903" xr:uid="{F527D3C7-625E-48F9-8C8F-FEAA499C60A6}"/>
+    <hyperlink ref="I19" r:id="rId32" display="https://www.promptingguide.ai/" xr:uid="{B5E55C19-C7C6-4A53-8296-85A332B1F4B7}"/>
+    <hyperlink ref="I20" r:id="rId33" display="https://www.promptingguide.ai/" xr:uid="{43A050DF-487B-4345-9EED-F2E898F682A2}"/>
+    <hyperlink ref="I9" r:id="rId34" display="https://www.promptingguide.ai/" xr:uid="{7C472CB5-6FDE-4AC7-AFED-816029FC3A3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>